<commit_message>
Continuação do guia de arquitetura
</commit_message>
<xml_diff>
--- a/Documentos/Definição de Arquitetura/Guia Definicao da Arquitetura.xlsx
+++ b/Documentos/Definição de Arquitetura/Guia Definicao da Arquitetura.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lucas\bandtec\3 semetre\Potopj\Grupo07-Backup\Documentos\Definição de Arquitetura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59C767DE-5216-4D56-9F74-57F38DBDE2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EFA501-2F7E-4179-8F3C-C4228C2E5696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
   <si>
     <t>MECANISMO DE IMPLEMENTAÇÃO</t>
   </si>
@@ -171,24 +171,9 @@
     <t>Agente de Coleta</t>
   </si>
   <si>
-    <t>Exemplo: Web Service RESTAPI</t>
-  </si>
-  <si>
-    <t>Exemplo: TXT com info de erros, segurança, etc.</t>
-  </si>
-  <si>
-    <t>Exemplo: SDK para IoT</t>
-  </si>
-  <si>
-    <t>Exemplo: Azure DevOps</t>
-  </si>
-  <si>
     <t>Configuração da IDE de deploy automatizado</t>
   </si>
   <si>
-    <t>Exemplo: Token ou SSO Com Google</t>
-  </si>
-  <si>
     <t>Integração contínua</t>
   </si>
   <si>
@@ -207,33 +192,9 @@
     <t>Windows, Linux, MacOs, Todos navegadores</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Java</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, ? IIS ? Tomcat ?</t>
-    </r>
-  </si>
-  <si>
     <t>SCRUM</t>
   </si>
   <si>
-    <t>Notion, Word, Excell, Canva</t>
-  </si>
-  <si>
     <t>Planner</t>
   </si>
   <si>
@@ -246,29 +207,6 @@
     <t xml:space="preserve">Definido que deve ser o GITHUB do Grupo de PI </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">? TesteCase </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>+ Ferramenta ? Jmeter</t>
-    </r>
-  </si>
-  <si>
     <t>React HTML, CSS, JS</t>
   </si>
   <si>
@@ -279,13 +217,25 @@
   </si>
   <si>
     <t>Azure SQL Server</t>
+  </si>
+  <si>
+    <t>Java 11</t>
+  </si>
+  <si>
+    <t>Em desenvolvimento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chat </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Word, Excell, Canva</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,14 +292,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -499,16 +441,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -517,6 +449,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -799,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036DB22A-6FFA-4CD0-A3AA-AF0DD32AFF0D}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -824,7 +766,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="23" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -834,35 +776,35 @@
         <v>2</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="26" t="s">
-        <v>48</v>
+      <c r="D3" s="16" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="26" t="s">
-        <v>49</v>
+      <c r="D4" s="22" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
@@ -870,23 +812,23 @@
         <v>4</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="26" t="s">
-        <v>50</v>
+      <c r="D6" s="22" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="2" t="s">
         <v>38</v>
       </c>
@@ -894,11 +836,11 @@
         <v>39</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
@@ -906,47 +848,47 @@
         <v>35</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="25" t="s">
-        <v>53</v>
+      <c r="D11" s="21" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -956,11 +898,11 @@
         <v>15</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
@@ -968,23 +910,23 @@
         <v>16</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="22" t="s">
-        <v>60</v>
+      <c r="D15" s="26" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
@@ -992,11 +934,11 @@
         <v>40</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="8" t="s">
         <v>29</v>
       </c>
@@ -1004,11 +946,11 @@
         <v>41</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="23" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -1017,12 +959,12 @@
       <c r="C19" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="23" t="s">
-        <v>61</v>
+      <c r="D19" s="19" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="1" t="s">
         <v>24</v>
       </c>
@@ -1030,11 +972,11 @@
         <v>42</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
+      <c r="A21" s="24"/>
       <c r="B21" s="1" t="s">
         <v>25</v>
       </c>
@@ -1042,11 +984,11 @@
         <v>43</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
@@ -1054,11 +996,11 @@
         <v>27</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
@@ -1066,11 +1008,11 @@
         <v>46</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="2" t="s">
         <v>18</v>
       </c>
@@ -1078,19 +1020,19 @@
         <v>31</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="24" t="s">
-        <v>67</v>
+      <c r="D25" s="20" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>